<commit_message>
feat: add tech stack file
</commit_message>
<xml_diff>
--- a/Document/Web前端项目进度.xlsx
+++ b/Document/Web前端项目进度.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>张雨生</t>
   </si>
@@ -95,10 +95,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -122,7 +122,129 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,128 +258,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -304,7 +304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.8"/>
+        <fgColor theme="6" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,187 +322,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,6 +525,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -540,15 +555,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -560,30 +566,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,6 +599,24 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -630,10 +630,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -642,133 +642,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1159,9 +1159,9 @@
   <dimension ref="B1:AB52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1282,13 +1282,13 @@
       <c r="E5" s="7"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" ht="14.25" hidden="1" outlineLevel="1" spans="3:14">
+    <row r="6" ht="14.25" hidden="1" outlineLevel="1" spans="3:13">
       <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="N6" s="1"/>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" ht="14.25" collapsed="1" spans="2:5">
       <c r="B7" s="6" t="s">
@@ -1322,13 +1322,13 @@
       <c r="E10" s="7"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" ht="14.25" hidden="1" outlineLevel="1" spans="3:14">
+    <row r="11" ht="14.25" hidden="1" outlineLevel="1" spans="3:13">
       <c r="C11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="N11" s="2"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" ht="14.25" collapsed="1" spans="2:5">
       <c r="B12" s="8" t="s">
@@ -1395,69 +1395,73 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" ht="14.25" spans="2:2">
-      <c r="B24" s="7" t="s">
+    <row r="24" ht="14.25" collapsed="1" spans="2:2">
+      <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="25" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C25" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" ht="14.25" outlineLevel="1" spans="3:3">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C26" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" ht="14.25" outlineLevel="1" spans="3:3">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C27" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" ht="14.25" outlineLevel="1" spans="3:3">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C28" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" ht="14.25" collapsed="1" spans="2:2">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" ht="14.25" spans="2:2">
       <c r="B29" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="30" ht="14.25" outlineLevel="1" spans="3:3">
       <c r="C30" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="31" ht="14.25" outlineLevel="1" spans="3:3">
       <c r="C31" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="32" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="32" ht="14.25" outlineLevel="1" spans="3:3">
       <c r="C32" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="33" ht="14.25" outlineLevel="1" spans="3:3">
       <c r="C33" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="34" ht="14.25" outlineLevel="1" spans="3:3">
       <c r="C34" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" ht="14.25" hidden="1" outlineLevel="1" spans="3:25">
+    <row r="35" ht="14.25" outlineLevel="1" spans="3:25">
       <c r="C35" s="7" t="s">
         <v>8</v>
       </c>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" ht="14.25" spans="2:3">
-      <c r="B36" s="9" t="s">
+    <row r="36" ht="14.25" collapsed="1" spans="2:3">
+      <c r="B36" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C36" s="7"/>
@@ -1478,48 +1482,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" ht="14.25" hidden="1" outlineLevel="1" spans="3:3">
+    <row r="40" ht="14.25" hidden="1" outlineLevel="1" spans="3:13">
       <c r="C40" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" ht="14.25" outlineLevel="1" spans="2:3">
+      <c r="M40" s="2"/>
+    </row>
+    <row r="41" ht="14.25" collapsed="1" spans="2:3">
       <c r="B41" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="7"/>
     </row>
-    <row r="42" ht="14.25" outlineLevel="1" spans="3:12">
+    <row r="42" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C42" s="7" t="s">
         <v>23</v>
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" ht="14.25" outlineLevel="1" spans="3:12">
+    <row r="43" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
       <c r="C43" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" ht="14.25" outlineLevel="1" spans="3:3">
-      <c r="C44" s="7"/>
-    </row>
-    <row r="45" ht="14.25" outlineLevel="1" spans="3:3">
-      <c r="C45" s="7"/>
-    </row>
-    <row r="46" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="44" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
+      <c r="C44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" ht="14.25" hidden="1" outlineLevel="1" spans="3:12">
+      <c r="C45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" ht="14.25" spans="3:3">
       <c r="C46" s="7"/>
     </row>
-    <row r="47" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="47" ht="14.25" spans="3:3">
       <c r="C47" s="7"/>
     </row>
-    <row r="48" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="48" ht="14.25" spans="3:3">
       <c r="C48" s="7"/>
     </row>
-    <row r="49" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="49" ht="14.25" spans="3:3">
       <c r="C49" s="7"/>
     </row>
-    <row r="50" ht="14.25" outlineLevel="1" spans="3:3">
+    <row r="50" ht="14.25" spans="3:3">
       <c r="C50" s="7"/>
     </row>
     <row r="52" ht="16.5" spans="2:21">

</xml_diff>